<commit_message>
Replicating the question format
</commit_message>
<xml_diff>
--- a/questions/2018_questions_yourname.xlsx
+++ b/questions/2018_questions_yourname.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HOME/Projects/twalve.github.io/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF9679C5-A688-884E-9508-AE70883D8DA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A731BCA-522F-B042-A9A3-2E04E67875E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{DC0E3E98-0B25-5544-B40F-1E7BD5276B11}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16420" activeTab="4" xr2:uid="{DC0E3E98-0B25-5544-B40F-1E7BD5276B11}"/>
   </bookViews>
   <sheets>
     <sheet name="Easiest" sheetId="5" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Hardest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -434,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B529B3-FA75-E541-AD3C-79D4404C5685}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,50 +443,50 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -499,53 +496,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A176AF-2525-8D44-AA4C-AC7CA0AC0DB3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D70AA0A-30B8-524B-88E0-C1DCB5ED21A9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB7D1C-0189-FF48-9A24-D8E3CAD93047}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9461A63-EA2C-E844-A9F6-337FCF8C98FC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="97.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D70AA0A-30B8-524B-88E0-C1DCB5ED21A9}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="97.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB7D1C-0189-FF48-9A24-D8E3CAD93047}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="97.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9461A63-EA2C-E844-A9F6-337FCF8C98FC}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="97.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a Hardest Question and formating the sheets
</commit_message>
<xml_diff>
--- a/questions/2018_questions_yourname.xlsx
+++ b/questions/2018_questions_yourname.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HOME/Projects/twalve.github.io/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A731BCA-522F-B042-A9A3-2E04E67875E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA346B12-1E54-5C45-837E-C192E7DFE517}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16420" activeTab="4" xr2:uid="{DC0E3E98-0B25-5544-B40F-1E7BD5276B11}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -70,13 +70,33 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>let a = 5;
+function first() {
+  a += 1;
+  return a;
+}
+function second() {
+  alert(first());
+}
+// What is alerted when I call `second()`?</t>
+  </si>
+  <si>
+    <t>None of these</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +110,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,9 +137,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,61 +466,110 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="97.5" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="181" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="26">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="26">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="26">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="26">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="26">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A176AF-2525-8D44-AA4C-AC7CA0AC0DB3}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="97.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="3" customFormat="1" ht="182" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A6" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -494,46 +577,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A176AF-2525-8D44-AA4C-AC7CA0AC0DB3}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D70AA0A-30B8-524B-88E0-C1DCB5ED21A9}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="97.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="3" customFormat="1" ht="182" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -543,46 +626,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D70AA0A-30B8-524B-88E0-C1DCB5ED21A9}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB7D1C-0189-FF48-9A24-D8E3CAD93047}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="97.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="3" customFormat="1" ht="182" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" s="1" customFormat="1" ht="26">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -592,97 +675,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB7D1C-0189-FF48-9A24-D8E3CAD93047}">
-  <dimension ref="A1:A6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9461A63-EA2C-E844-A9F6-337FCF8C98FC}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="97.5" customWidth="1"/>
+    <col min="2" max="2" width="97.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="179" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="26">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="26">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="26">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="26">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="26">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9461A63-EA2C-E844-A9F6-337FCF8C98FC}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="97.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>